<commit_message>
[CSV] StaffInfo 오타 수정
</commit_message>
<xml_diff>
--- a/Design/Tables/StaffInfo.xlsx
+++ b/Design/Tables/StaffInfo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B701EBF-C54E-4184-9E85-AF40D047705D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432E1B1D-84E1-42B0-8D0B-EFB7ADD54991}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,10 +30,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>String</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Staff</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -71,6 +67,10 @@
   </si>
   <si>
     <t>IsPay</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -399,7 +399,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -412,13 +412,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -426,13 +426,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -440,7 +440,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -454,7 +454,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
@@ -468,7 +468,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -482,7 +482,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
@@ -496,7 +496,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -510,7 +510,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>

</xml_diff>